<commit_message>
belt_control software: add the test mode with the key
</commit_message>
<xml_diff>
--- a/Send_Medicine_Motor/hardware/Send_Medicine_Motor.xlsx
+++ b/Send_Medicine_Motor/hardware/Send_Medicine_Motor.xlsx
@@ -3,11 +3,6 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\program\2016year\myprogram_2016year\Send_Medicine_Motor\hardware\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-30" yWindow="75" windowWidth="15165" windowHeight="8820"/>
   </bookViews>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="133">
   <si>
     <t>Approved</t>
   </si>
@@ -95,7 +90,7 @@
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>2017/4/27</t>
+    <t>2017/5/9</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
@@ -111,7 +106,7 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>15:44:16</t>
+    <t>14:17:03</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
@@ -398,6 +393,14 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>Send_Medicine_Motor.PrjPcb</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>None</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Send_Medicine_Motor.PcbDoc</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
@@ -406,19 +409,19 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>Bill of Materials For PCB Document [Send_Medicine_Motor.PcbDoc]</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>273</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>15:44:16</t>
+    <t>14:17:03</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>2017/4/27</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>2017/4/27 15:44:16</t>
+    <t>2017/5/9 14:17:03</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
@@ -431,6 +434,10 @@
   </si>
   <si>
     <t>BOM</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bill of Materials</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
 </sst>
@@ -1436,8 +1443,8 @@
   </sheetPr>
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD34"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1542,11 +1549,11 @@
       </c>
       <c r="B8" s="13">
         <f ca="1">TODAY()</f>
-        <v>42852</v>
+        <v>42864</v>
       </c>
       <c r="C8" s="14">
         <f ca="1">NOW()</f>
-        <v>42852.657700810189</v>
+        <v>42864.595253935186</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="5"/>
@@ -1584,7 +1591,7 @@
     </row>
     <row r="11" spans="1:7" s="15" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A11" s="74">
-        <f t="shared" ref="A11:A46" si="0">ROW(A11) - ROW($A$10)</f>
+        <f>ROW(A11) - ROW($A$10)</f>
         <v>1</v>
       </c>
       <c r="B11" s="82" t="s">
@@ -1605,7 +1612,7 @@
     </row>
     <row r="12" spans="1:7" s="15" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A12) - ROW($A$10)</f>
         <v>2</v>
       </c>
       <c r="B12" s="82" t="s">
@@ -1626,7 +1633,7 @@
     </row>
     <row r="13" spans="1:7" s="15" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A13) - ROW($A$10)</f>
         <v>3</v>
       </c>
       <c r="B13" s="82" t="s">
@@ -1647,7 +1654,7 @@
     </row>
     <row r="14" spans="1:7" s="15" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A14) - ROW($A$10)</f>
         <v>4</v>
       </c>
       <c r="B14" s="82" t="s">
@@ -1668,7 +1675,7 @@
     </row>
     <row r="15" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A15) - ROW($A$10)</f>
         <v>5</v>
       </c>
       <c r="B15" s="82" t="s">
@@ -1689,7 +1696,7 @@
     </row>
     <row r="16" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A16) - ROW($A$10)</f>
         <v>6</v>
       </c>
       <c r="B16" s="82" t="s">
@@ -1710,7 +1717,7 @@
     </row>
     <row r="17" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A17) - ROW($A$10)</f>
         <v>7</v>
       </c>
       <c r="B17" s="82" t="s">
@@ -1731,7 +1738,7 @@
     </row>
     <row r="18" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A18) - ROW($A$10)</f>
         <v>8</v>
       </c>
       <c r="B18" s="82" t="s">
@@ -1752,7 +1759,7 @@
     </row>
     <row r="19" spans="1:6" s="15" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A19) - ROW($A$10)</f>
         <v>9</v>
       </c>
       <c r="B19" s="82" t="s">
@@ -1773,7 +1780,7 @@
     </row>
     <row r="20" spans="1:6" s="15" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A20) - ROW($A$10)</f>
         <v>10</v>
       </c>
       <c r="B20" s="82" t="s">
@@ -1794,7 +1801,7 @@
     </row>
     <row r="21" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A21) - ROW($A$10)</f>
         <v>11</v>
       </c>
       <c r="B21" s="82" t="s">
@@ -1815,7 +1822,7 @@
     </row>
     <row r="22" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A22) - ROW($A$10)</f>
         <v>12</v>
       </c>
       <c r="B22" s="82" t="s">
@@ -1836,7 +1843,7 @@
     </row>
     <row r="23" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A23) - ROW($A$10)</f>
         <v>13</v>
       </c>
       <c r="B23" s="82" t="s">
@@ -1857,7 +1864,7 @@
     </row>
     <row r="24" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A24) - ROW($A$10)</f>
         <v>14</v>
       </c>
       <c r="B24" s="82" t="s">
@@ -1878,7 +1885,7 @@
     </row>
     <row r="25" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A25) - ROW($A$10)</f>
         <v>15</v>
       </c>
       <c r="B25" s="82" t="s">
@@ -1899,7 +1906,7 @@
     </row>
     <row r="26" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A26) - ROW($A$10)</f>
         <v>16</v>
       </c>
       <c r="B26" s="82" t="s">
@@ -1920,7 +1927,7 @@
     </row>
     <row r="27" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A27) - ROW($A$10)</f>
         <v>17</v>
       </c>
       <c r="B27" s="82" t="s">
@@ -1941,7 +1948,7 @@
     </row>
     <row r="28" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A28) - ROW($A$10)</f>
         <v>18</v>
       </c>
       <c r="B28" s="82" t="s">
@@ -1962,7 +1969,7 @@
     </row>
     <row r="29" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A29) - ROW($A$10)</f>
         <v>19</v>
       </c>
       <c r="B29" s="82" t="s">
@@ -1983,7 +1990,7 @@
     </row>
     <row r="30" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A30) - ROW($A$10)</f>
         <v>20</v>
       </c>
       <c r="B30" s="82" t="s">
@@ -2004,7 +2011,7 @@
     </row>
     <row r="31" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A31) - ROW($A$10)</f>
         <v>21</v>
       </c>
       <c r="B31" s="82" t="s">
@@ -2025,7 +2032,7 @@
     </row>
     <row r="32" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A32) - ROW($A$10)</f>
         <v>22</v>
       </c>
       <c r="B32" s="82" t="s">
@@ -2046,7 +2053,7 @@
     </row>
     <row r="33" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A33) - ROW($A$10)</f>
         <v>23</v>
       </c>
       <c r="B33" s="82" t="s">
@@ -2067,7 +2074,7 @@
     </row>
     <row r="34" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A34) - ROW($A$10)</f>
         <v>24</v>
       </c>
       <c r="B34" s="82" t="s">
@@ -2088,7 +2095,7 @@
     </row>
     <row r="35" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A35) - ROW($A$10)</f>
         <v>25</v>
       </c>
       <c r="B35" s="82" t="s">
@@ -2109,7 +2116,7 @@
     </row>
     <row r="36" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A36) - ROW($A$10)</f>
         <v>26</v>
       </c>
       <c r="B36" s="82" t="s">
@@ -2130,7 +2137,7 @@
     </row>
     <row r="37" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A37) - ROW($A$10)</f>
         <v>27</v>
       </c>
       <c r="B37" s="82" t="s">
@@ -2151,7 +2158,7 @@
     </row>
     <row r="38" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A38) - ROW($A$10)</f>
         <v>28</v>
       </c>
       <c r="B38" s="82" t="s">
@@ -2172,7 +2179,7 @@
     </row>
     <row r="39" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A39) - ROW($A$10)</f>
         <v>29</v>
       </c>
       <c r="B39" s="82" t="s">
@@ -2191,9 +2198,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="15" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A40) - ROW($A$10)</f>
         <v>30</v>
       </c>
       <c r="B40" s="82" t="s">
@@ -2214,7 +2221,7 @@
     </row>
     <row r="41" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A41) - ROW($A$10)</f>
         <v>31</v>
       </c>
       <c r="B41" s="82" t="s">
@@ -2235,7 +2242,7 @@
     </row>
     <row r="42" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A42) - ROW($A$10)</f>
         <v>32</v>
       </c>
       <c r="B42" s="82" t="s">
@@ -2256,7 +2263,7 @@
     </row>
     <row r="43" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A43) - ROW($A$10)</f>
         <v>33</v>
       </c>
       <c r="B43" s="82" t="s">
@@ -2277,7 +2284,7 @@
     </row>
     <row r="44" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A44) - ROW($A$10)</f>
         <v>34</v>
       </c>
       <c r="B44" s="82" t="s">
@@ -2298,7 +2305,7 @@
     </row>
     <row r="45" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A45) - ROW($A$10)</f>
         <v>35</v>
       </c>
       <c r="B45" s="82" t="s">
@@ -2319,7 +2326,7 @@
     </row>
     <row r="46" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="74">
-        <f t="shared" si="0"/>
+        <f>ROW(A46) - ROW($A$10)</f>
         <v>36</v>
       </c>
       <c r="B46" s="82" t="s">
@@ -2473,7 +2480,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="86" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="19" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2481,7 +2488,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="87" t="s">
-        <v>27</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="19" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2489,7 +2496,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="86" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:2" s="19" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2497,7 +2504,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="87" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="19" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2505,7 +2512,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="86" t="s">
-        <v>29</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="19" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2513,7 +2520,7 @@
         <v>13</v>
       </c>
       <c r="B7" s="87" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="19" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2521,7 +2528,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="86" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:2" s="19" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2529,7 +2536,7 @@
         <v>15</v>
       </c>
       <c r="B9" s="87" t="s">
-        <v>125</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="19" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2537,7 +2544,7 @@
         <v>17</v>
       </c>
       <c r="B10" s="86" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="19" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2545,7 +2552,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="87" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:2" s="19" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2553,7 +2560,7 @@
         <v>18</v>
       </c>
       <c r="B12" s="86" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="19" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2561,7 +2568,7 @@
         <v>19</v>
       </c>
       <c r="B13" s="87" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="19" customFormat="1" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2569,7 +2576,7 @@
         <v>20</v>
       </c>
       <c r="B14" s="88" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>